<commit_message>
Updates - Including Table Updates
</commit_message>
<xml_diff>
--- a/2 - RiverWare Modeling/Hydrology/MI+AG.xlsx
+++ b/2 - RiverWare Modeling/Hydrology/MI+AG.xlsx
@@ -8,24 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Documents\GitHub\WeberBasinVulnerability\WeberBasinVulnerability\2 - RiverWare Modeling\Hydrology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EBE7B46-BD28-4E1F-8463-E6016CD6DEF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BD5749-4D4C-4E23-A9DB-EC15ABCE4225}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="991" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Trace1" sheetId="1" r:id="rId1"/>
-    <sheet name="Trace2" sheetId="2" r:id="rId2"/>
-    <sheet name="Trace3" sheetId="3" r:id="rId3"/>
-    <sheet name="Trace4" sheetId="4" r:id="rId4"/>
-    <sheet name="Trace5" sheetId="5" r:id="rId5"/>
-    <sheet name="Trace6" sheetId="6" r:id="rId6"/>
+    <sheet name="Trace0" sheetId="1" r:id="rId1"/>
+    <sheet name="Trace1" sheetId="2" r:id="rId2"/>
+    <sheet name="Trace2" sheetId="18" r:id="rId3"/>
+    <sheet name="Trace3" sheetId="4" r:id="rId4"/>
+    <sheet name="Trace4" sheetId="5" r:id="rId5"/>
+    <sheet name="Trace5" sheetId="27" r:id="rId6"/>
+    <sheet name="Trace6" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="23">
   <si>
     <t>SA1</t>
   </si>
@@ -85,6 +86,9 @@
   </si>
   <si>
     <t>SA20</t>
+  </si>
+  <si>
+    <t>!label!header!</t>
   </si>
   <si>
     <t>Demand Data.AnnualDemands</t>
@@ -97,6 +101,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode=";;;"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -126,8 +133,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,18 +437,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>21</v>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -453,7 +469,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>31681.743579397</v>
+        <v>31300</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -461,7 +477,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>10931.7198293127</v>
+        <v>10800</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -469,7 +485,7 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>9044.1817783549395</v>
+        <v>9000</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -477,7 +493,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>6330.9272448484598</v>
+        <v>6300</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -485,7 +501,7 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>21806.527176700201</v>
+        <v>21700</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -493,7 +509,7 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>6680.4954512466502</v>
+        <v>6600</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -501,7 +517,7 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>10853.018134025901</v>
+        <v>10800</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -509,7 +525,7 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>1507.3636297258199</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -517,7 +533,7 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>92888.6433827867</v>
+        <v>88600</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -525,7 +541,7 @@
         <v>10</v>
       </c>
       <c r="B13">
-        <v>64896.241821608302</v>
+        <v>61900</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -533,7 +549,7 @@
         <v>11</v>
       </c>
       <c r="B14">
-        <v>27394.692609923699</v>
+        <v>26800</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -541,7 +557,7 @@
         <v>12</v>
       </c>
       <c r="B15">
-        <v>31381.233698681299</v>
+        <v>30700</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -549,7 +565,7 @@
         <v>13</v>
       </c>
       <c r="B16">
-        <v>23817.027530269501</v>
+        <v>23300</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -557,7 +573,7 @@
         <v>14</v>
       </c>
       <c r="B17">
-        <v>75028.747670462704</v>
+        <v>73400</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -565,7 +581,7 @@
         <v>15</v>
       </c>
       <c r="B18">
-        <v>19421.610432408601</v>
+        <v>19000</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -573,7 +589,7 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <v>61842.496376880001</v>
+        <v>60500</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -581,7 +597,7 @@
         <v>17</v>
       </c>
       <c r="B20">
-        <v>9488.8148702581802</v>
+        <v>12800</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -589,7 +605,7 @@
         <v>18</v>
       </c>
       <c r="B21">
-        <v>18603.858414201899</v>
+        <v>18200</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -610,18 +626,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>21</v>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -637,7 +658,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>30947.536507588698</v>
+        <v>31681.743579397</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -645,7 +666,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>10678.383203896499</v>
+        <v>10931.7198293127</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -653,7 +674,7 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>8883.0450335063906</v>
+        <v>9044.1817783549395</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -661,7 +682,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>6218.13152345448</v>
+        <v>6330.9272448484598</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -669,7 +690,7 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>21418.008580787598</v>
+        <v>21806.527176700201</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -677,7 +698,7 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>6525.6786246033898</v>
+        <v>6680.4954512466502</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -685,7 +706,7 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>10659.654040207701</v>
+        <v>10853.018134025901</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -693,7 +714,7 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>1480.5075055844</v>
+        <v>1507.3636297258199</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -701,7 +722,7 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>89046.643462849097</v>
+        <v>92888.6433827867</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -709,7 +730,7 @@
         <v>10</v>
       </c>
       <c r="B13">
-        <v>62212.0454892817</v>
+        <v>64896.241821608302</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -717,7 +738,7 @@
         <v>11</v>
       </c>
       <c r="B14">
-        <v>25643.0749329061</v>
+        <v>27394.692609923699</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -725,7 +746,7 @@
         <v>12</v>
       </c>
       <c r="B15">
-        <v>29374.7164343365</v>
+        <v>31381.233698681299</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -733,7 +754,7 @@
         <v>13</v>
       </c>
       <c r="B16">
-        <v>22294.165893160902</v>
+        <v>23817.027530269501</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -741,7 +762,7 @@
         <v>14</v>
       </c>
       <c r="B17">
-        <v>70231.406719227904</v>
+        <v>75028.747670462704</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -749,7 +770,7 @@
         <v>15</v>
       </c>
       <c r="B18">
-        <v>18179.7919300453</v>
+        <v>19421.610432408601</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -757,7 +778,7 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <v>57888.284829881399</v>
+        <v>61842.496376880001</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -765,7 +786,7 @@
         <v>17</v>
       </c>
       <c r="B20">
-        <v>4112.7512507066003</v>
+        <v>9488.8148702581802</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -773,7 +794,7 @@
         <v>18</v>
       </c>
       <c r="B21">
-        <v>17414.327006675001</v>
+        <v>18603.858414201899</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -791,21 +812,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>21</v>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -821,7 +847,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>28829.6512914665</v>
+        <v>30947.536507588698</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -829,7 +855,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>9947.6113082376796</v>
+        <v>10678.383203896499</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -837,7 +863,7 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>8668.7280083851892</v>
+        <v>8883.0450335063906</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -845,7 +871,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>6068.1096058696303</v>
+        <v>6218.13152345448</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -853,7 +879,7 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>20901.266420217598</v>
+        <v>21418.008580787598</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -861,7 +887,7 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>6079.0957994785704</v>
+        <v>6525.6786246033898</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -869,7 +895,7 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>10402.473610062199</v>
+        <v>10659.654040207701</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -877,7 +903,7 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>1444.78800139753</v>
+        <v>1480.5075055844</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -885,7 +911,7 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>106672.61314313899</v>
+        <v>89046.643462849097</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -893,7 +919,7 @@
         <v>10</v>
       </c>
       <c r="B13">
-        <v>74526.351620319401</v>
+        <v>62212.0454892817</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -901,7 +927,7 @@
         <v>11</v>
       </c>
       <c r="B14">
-        <v>24621.7151297768</v>
+        <v>25643.0749329061</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -909,7 +935,7 @@
         <v>12</v>
       </c>
       <c r="B15">
-        <v>28204.725913587499</v>
+        <v>29374.7164343365</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -917,7 +943,7 @@
         <v>13</v>
       </c>
       <c r="B16">
-        <v>21406.192631484901</v>
+        <v>22294.165893160902</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -925,7 +951,7 @@
         <v>14</v>
       </c>
       <c r="B17">
-        <v>67434.100392746594</v>
+        <v>70231.406719227904</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -933,7 +959,7 @@
         <v>15</v>
       </c>
       <c r="B18">
-        <v>17455.693562155</v>
+        <v>18179.7919300453</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -941,7 +967,7 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <v>55582.603184757099</v>
+        <v>57888.284829881399</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -949,7 +975,7 @@
         <v>17</v>
       </c>
       <c r="B20">
-        <v>977.99571330001004</v>
+        <v>4112.7512507066003</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -957,7 +983,7 @@
         <v>18</v>
       </c>
       <c r="B21">
-        <v>16720.7169911169</v>
+        <v>17414.327006675001</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -978,18 +1004,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>21</v>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1005,7 +1036,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>28518.644557815802</v>
+        <v>28829.6512914665</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1013,7 +1044,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>9840.2990806520902</v>
+        <v>9947.6113082376796</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1021,7 +1052,7 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>8795.3590655888092</v>
+        <v>8668.7280083851892</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1029,7 +1060,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>6156.7513459121701</v>
+        <v>6068.1096058696303</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1037,7 +1068,7 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>21206.587969253</v>
+        <v>20901.266420217598</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1045,7 +1076,7 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>6013.51610484295</v>
+        <v>6079.0957994785704</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1053,7 +1084,7 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>10554.4308787066</v>
+        <v>10402.473610062199</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1061,7 +1092,7 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>1465.89317759814</v>
+        <v>1444.78800139753</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1069,7 +1100,7 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>68875.343333618497</v>
+        <v>106672.61314313899</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1077,7 +1108,7 @@
         <v>10</v>
       </c>
       <c r="B13">
-        <v>48119.455444141997</v>
+        <v>74526.351620319401</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1085,7 +1116,7 @@
         <v>11</v>
       </c>
       <c r="B14">
-        <v>24110.075449917498</v>
+        <v>24621.7151297768</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1093,7 +1124,7 @@
         <v>12</v>
       </c>
       <c r="B15">
-        <v>27618.6312056891</v>
+        <v>28204.725913587499</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1101,7 +1132,7 @@
         <v>13</v>
       </c>
       <c r="B16">
-        <v>20961.3715665327</v>
+        <v>21406.192631484901</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1109,7 +1140,7 @@
         <v>14</v>
       </c>
       <c r="B17">
-        <v>66032.818582983004</v>
+        <v>67434.100392746594</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1117,7 +1148,7 @@
         <v>15</v>
       </c>
       <c r="B18">
-        <v>17092.963938374302</v>
+        <v>17455.693562155</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1125,7 +1156,7 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <v>54427.595698507801</v>
+        <v>55582.603184757099</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1133,7 +1164,7 @@
         <v>17</v>
       </c>
       <c r="B20">
-        <v>9473.6364234191806</v>
+        <v>977.99571330001004</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1141,7 +1172,7 @@
         <v>18</v>
       </c>
       <c r="B21">
-        <v>16373.260193600699</v>
+        <v>16720.7169911169</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1162,18 +1193,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>21</v>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1189,7 +1225,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>26715.024646942598</v>
+        <v>28518.644557815802</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1197,7 +1233,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>9217.9637759418601</v>
+        <v>9840.2990806520902</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1205,7 +1241,7 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>8391.2459169097292</v>
+        <v>8795.3590655888092</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1213,7 +1249,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>5873.8721418368104</v>
+        <v>6156.7513459121701</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1221,7 +1257,7 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>20232.226266326801</v>
+        <v>21206.587969253</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1229,7 +1265,7 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>5633.2000852977999</v>
+        <v>6013.51610484295</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1237,7 +1273,7 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>10069.495100291701</v>
+        <v>10554.4308787066</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1245,7 +1281,7 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>1398.54098615162</v>
+        <v>1465.89317759814</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1253,7 +1289,7 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>62783.614774734102</v>
+        <v>68875.343333618497</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1261,7 +1297,7 @@
         <v>10</v>
       </c>
       <c r="B13">
-        <v>43863.496101083903</v>
+        <v>48119.455444141997</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1269,7 +1305,7 @@
         <v>11</v>
       </c>
       <c r="B14">
-        <v>19718.211753909101</v>
+        <v>24110.075449917498</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1277,7 +1313,7 @@
         <v>12</v>
       </c>
       <c r="B15">
-        <v>22587.653016604701</v>
+        <v>27618.6312056891</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1285,7 +1321,7 @@
         <v>13</v>
       </c>
       <c r="B16">
-        <v>17143.072159182098</v>
+        <v>20961.3715665327</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1293,7 +1329,7 @@
         <v>14</v>
       </c>
       <c r="B17">
-        <v>54004.3560722732</v>
+        <v>66032.818582983004</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1301,7 +1337,7 @@
         <v>15</v>
       </c>
       <c r="B18">
-        <v>13979.329228517599</v>
+        <v>17092.963938374302</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1309,7 +1345,7 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <v>44513.127280279798</v>
+        <v>54427.595698507801</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1317,7 +1353,7 @@
         <v>17</v>
       </c>
       <c r="B20">
-        <v>4083.7040337543199</v>
+        <v>9473.6364234191806</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1325,7 +1361,7 @@
         <v>18</v>
       </c>
       <c r="B21">
-        <v>13390.72589258</v>
+        <v>16373.260193600699</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1343,21 +1379,215 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>35500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>26715.024646942598</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>9217.9637759418601</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>8391.2459169097292</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>5873.8721418368104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>20232.226266326801</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>5633.2000852977999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>10069.495100291701</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>1398.54098615162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>62783.614774734102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>43863.496101083903</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>19718.211753909101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>22587.653016604701</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>17143.072159182098</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>54004.3560722732</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>13979.329228517599</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>44513.127280279798</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>4083.7040337543199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>13390.72589258</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Revamp on Demand Scenarios
Demand Scenarios upgraded to include multiple Ag Conversion Factors
</commit_message>
<xml_diff>
--- a/2 - RiverWare Modeling/Hydrology/MI+AG.xlsx
+++ b/2 - RiverWare Modeling/Hydrology/MI+AG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Documents\GitHub\WeberBasinVulnerability\WeberBasinVulnerability\2 - RiverWare Modeling\Hydrology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BD5749-4D4C-4E23-A9DB-EC15ABCE4225}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE01B3A5-6D6B-494B-8466-D338E636BC12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="991" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="991" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trace0" sheetId="1" r:id="rId1"/>
@@ -627,7 +627,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B3" sqref="B3:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,7 +658,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>31681.743579397</v>
+        <v>28732.420962278102</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -666,7 +666,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>10931.7198293127</v>
+        <v>9914.0621850671996</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -674,7 +674,7 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>9044.1817783549395</v>
+        <v>8820.1008614675793</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -682,7 +682,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>6330.9272448484598</v>
+        <v>6174.0706030273004</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -690,7 +690,7 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>21806.527176700201</v>
+        <v>21266.243188205201</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -698,7 +698,7 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>6680.4954512466502</v>
+        <v>6058.5935575410704</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -706,7 +706,7 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>10853.018134025901</v>
+        <v>10584.121033761099</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -714,7 +714,7 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>1507.3636297258199</v>
+        <v>1470.0168102446</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -722,7 +722,7 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>92888.6433827867</v>
+        <v>71276.983627979003</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -730,7 +730,7 @@
         <v>10</v>
       </c>
       <c r="B13">
-        <v>64896.241821608302</v>
+        <v>49797.350864242697</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -738,7 +738,7 @@
         <v>11</v>
       </c>
       <c r="B14">
-        <v>27394.692609923699</v>
+        <v>24443.103311474799</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -746,7 +746,7 @@
         <v>12</v>
       </c>
       <c r="B15">
-        <v>31381.233698681299</v>
+        <v>28000.1220769506</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -754,7 +754,7 @@
         <v>13</v>
       </c>
       <c r="B16">
-        <v>23817.027530269501</v>
+        <v>21250.906983483699</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -762,7 +762,7 @@
         <v>14</v>
       </c>
       <c r="B17">
-        <v>75028.747670462704</v>
+        <v>66944.917278442095</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -770,7 +770,7 @@
         <v>15</v>
       </c>
       <c r="B18">
-        <v>19421.610432408601</v>
+        <v>17329.065780523099</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -778,7 +778,7 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <v>61842.496376880001</v>
+        <v>55179.393669560603</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -786,7 +786,7 @@
         <v>17</v>
       </c>
       <c r="B20">
-        <v>9488.8148702581802</v>
+        <v>12788.081288257699</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -794,7 +794,7 @@
         <v>18</v>
       </c>
       <c r="B21">
-        <v>18603.858414201899</v>
+        <v>16599.420905553801</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -847,7 +847,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>30947.536507588698</v>
+        <v>31681.743579397</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -855,7 +855,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>10678.383203896499</v>
+        <v>10931.7198293127</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -863,7 +863,7 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>8883.0450335063906</v>
+        <v>9044.1817783549395</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -871,7 +871,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>6218.13152345448</v>
+        <v>6330.9272448484598</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -879,7 +879,7 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>21418.008580787598</v>
+        <v>21806.527176700201</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -887,7 +887,7 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>6525.6786246033898</v>
+        <v>6680.4954512466502</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -895,7 +895,7 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>10659.654040207701</v>
+        <v>10853.018134025901</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -903,7 +903,7 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>1480.5075055844</v>
+        <v>1507.3636297258199</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -911,7 +911,7 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>89046.643462849097</v>
+        <v>92888.6433827867</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -919,7 +919,7 @@
         <v>10</v>
       </c>
       <c r="B13">
-        <v>62212.0454892817</v>
+        <v>64896.241821608302</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -927,7 +927,7 @@
         <v>11</v>
       </c>
       <c r="B14">
-        <v>25643.0749329061</v>
+        <v>27394.692609923699</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -935,7 +935,7 @@
         <v>12</v>
       </c>
       <c r="B15">
-        <v>29374.7164343365</v>
+        <v>31381.233698681299</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -943,7 +943,7 @@
         <v>13</v>
       </c>
       <c r="B16">
-        <v>22294.165893160902</v>
+        <v>23817.027530269501</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -951,7 +951,7 @@
         <v>14</v>
       </c>
       <c r="B17">
-        <v>70231.406719227904</v>
+        <v>75028.747670462704</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -959,7 +959,7 @@
         <v>15</v>
       </c>
       <c r="B18">
-        <v>18179.7919300453</v>
+        <v>19421.610432408601</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -967,7 +967,7 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <v>57888.284829881399</v>
+        <v>61842.496376880001</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -975,7 +975,7 @@
         <v>17</v>
       </c>
       <c r="B20">
-        <v>4112.7512507066003</v>
+        <v>12802.08957378</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -983,7 +983,7 @@
         <v>18</v>
       </c>
       <c r="B21">
-        <v>17414.327006675001</v>
+        <v>18603.858414201899</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1004,7 +1004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:B22"/>
     </sheetView>
   </sheetViews>
@@ -1036,7 +1036,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>28829.6512914665</v>
+        <v>26090.740833122902</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1044,7 +1044,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>9947.6113082376796</v>
+        <v>9002.5559424194107</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1052,7 +1052,7 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>8668.7280083851892</v>
+        <v>8485.8609535813594</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1060,7 +1060,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>6068.1096058696303</v>
+        <v>5940.1026675069597</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1068,7 +1068,7 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>20901.266420217598</v>
+        <v>20460.353632523998</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1076,7 +1076,7 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>6079.0957994785704</v>
+        <v>5501.56196481186</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1084,7 +1084,7 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>10402.473610062199</v>
+        <v>10183.0331442976</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1092,7 +1092,7 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>1444.78800139753</v>
+        <v>1414.31015893023</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1100,7 +1100,7 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>106672.61314313899</v>
+        <v>54913.4886191677</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1108,7 +1108,7 @@
         <v>10</v>
       </c>
       <c r="B13">
-        <v>74526.351620319401</v>
+        <v>38365.067105265</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1116,7 +1116,7 @@
         <v>11</v>
       </c>
       <c r="B14">
-        <v>24621.7151297768</v>
+        <v>16995.8415208027</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1124,7 +1124,7 @@
         <v>12</v>
       </c>
       <c r="B15">
-        <v>28204.725913587499</v>
+        <v>19469.116965993999</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1132,7 +1132,7 @@
         <v>13</v>
       </c>
       <c r="B16">
-        <v>21406.192631484901</v>
+        <v>14776.2353520411</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1140,7 +1140,7 @@
         <v>14</v>
       </c>
       <c r="B17">
-        <v>67434.100392746594</v>
+        <v>46548.312224884699</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1148,7 +1148,7 @@
         <v>15</v>
       </c>
       <c r="B18">
-        <v>17455.693562155</v>
+        <v>12049.2906304197</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1156,7 +1156,7 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <v>55582.603184757099</v>
+        <v>38367.478060020803</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1164,7 +1164,7 @@
         <v>17</v>
       </c>
       <c r="B20">
-        <v>977.99571330001004</v>
+        <v>13377.5750928791</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1172,7 +1172,7 @@
         <v>18</v>
       </c>
       <c r="B21">
-        <v>16720.7169911169</v>
+        <v>11541.952077559999</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1194,7 +1194,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B22"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,7 +1225,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>28518.644557815802</v>
+        <v>31775.7574938656</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1233,7 +1233,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>9840.2990806520902</v>
+        <v>10964.159135263601</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1241,7 +1241,7 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>8795.3590655888092</v>
+        <v>9254.3888799342603</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1249,7 +1249,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>6156.7513459121701</v>
+        <v>6478.07221595398</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1257,7 +1257,7 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>21206.587969253</v>
+        <v>22313.3598549526</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1265,7 +1265,7 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>6013.51610484295</v>
+        <v>6700.3194715499503</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1273,7 +1273,7 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>10554.4308787066</v>
+        <v>11105.266655921099</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1281,7 +1281,7 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>1465.89317759814</v>
+        <v>1542.39814665571</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1289,7 +1289,7 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>68875.343333618497</v>
+        <v>89630.3043069251</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1297,7 +1297,7 @@
         <v>10</v>
       </c>
       <c r="B13">
-        <v>48119.455444141997</v>
+        <v>62619.8175688337</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1305,7 +1305,7 @@
         <v>11</v>
       </c>
       <c r="B14">
-        <v>24110.075449917498</v>
+        <v>26062.977655668499</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1313,7 +1313,7 @@
         <v>12</v>
       </c>
       <c r="B15">
-        <v>27618.6312056891</v>
+        <v>29855.724404068002</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1321,7 +1321,7 @@
         <v>13</v>
       </c>
       <c r="B16">
-        <v>20961.3715665327</v>
+        <v>22659.2305737715</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1329,7 +1329,7 @@
         <v>14</v>
       </c>
       <c r="B17">
-        <v>66032.818582983004</v>
+        <v>71381.438803211306</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1337,7 +1337,7 @@
         <v>15</v>
       </c>
       <c r="B18">
-        <v>17092.963938374302</v>
+        <v>18477.484158869302</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1345,7 +1345,7 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <v>54427.595698507801</v>
+        <v>58836.199558505301</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1353,7 +1353,7 @@
         <v>17</v>
       </c>
       <c r="B20">
-        <v>9473.6364234191806</v>
+        <v>13423.844797949299</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1361,7 +1361,7 @@
         <v>18</v>
       </c>
       <c r="B21">
-        <v>16373.260193600699</v>
+        <v>17699.484825864402</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1383,7 +1383,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B22"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1414,7 +1414,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>26715.024646942598</v>
+        <v>17754.571528347598</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1422,7 +1422,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>9217.9637759418601</v>
+        <v>6126.1780353403801</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1430,7 +1430,7 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>8391.2459169097292</v>
+        <v>7646.5753886840102</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1438,7 +1438,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>5873.8721418368104</v>
+        <v>5352.6027720788097</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1446,7 +1446,7 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>20232.226266326801</v>
+        <v>18436.742881604801</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1454,7 +1454,7 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>5633.2000852977999</v>
+        <v>3743.7754660413302</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1462,7 +1462,7 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>10069.495100291701</v>
+        <v>9175.8904664208094</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1470,7 +1470,7 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>1398.54098615162</v>
+        <v>1274.42923144734</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1478,7 +1478,7 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>62783.614774734102</v>
+        <v>65937.753117341097</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1486,7 +1486,7 @@
         <v>10</v>
       </c>
       <c r="B13">
-        <v>43863.496101083903</v>
+        <v>46067.120970241704</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1494,7 +1494,7 @@
         <v>11</v>
       </c>
       <c r="B14">
-        <v>19718.211753909101</v>
+        <v>14004.9075756615</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1502,7 +1502,7 @@
         <v>12</v>
       </c>
       <c r="B15">
-        <v>22587.653016604701</v>
+        <v>16042.935170627199</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1510,7 +1510,7 @@
         <v>13</v>
       </c>
       <c r="B16">
-        <v>17143.072159182098</v>
+        <v>12175.908451974399</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1518,7 +1518,7 @@
         <v>14</v>
       </c>
       <c r="B17">
-        <v>54004.3560722732</v>
+        <v>38356.724479610297</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1526,7 +1526,7 @@
         <v>15</v>
       </c>
       <c r="B18">
-        <v>13979.329228517599</v>
+        <v>9928.8523857301807</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1534,7 +1534,7 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <v>44513.127280279798</v>
+        <v>31615.556280877699</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1542,7 +1542,7 @@
         <v>17</v>
       </c>
       <c r="B20">
-        <v>4083.7040337543199</v>
+        <v>13728.132423462201</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1550,7 +1550,7 @@
         <v>18</v>
       </c>
       <c r="B21">
-        <v>13390.72589258</v>
+        <v>9510.7954431731196</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1571,8 +1571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1603,7 +1603,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>16958.147868001099</v>
+        <v>29202.3042101338</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1611,7 +1611,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>5851.3737052528104</v>
+        <v>10076.1944239439</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1619,7 +1619,7 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>7090.6778037744598</v>
+        <v>9153.5940514733302</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1627,7 +1627,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>4963.4744626421298</v>
+        <v>6407.5158360313399</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1635,7 +1635,7 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>17096.412037989499</v>
+        <v>22070.332324107902</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1643,7 +1643,7 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>3575.8394865433702</v>
+        <v>6157.6743701879404</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1651,7 +1651,7 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>8508.8133645293401</v>
+        <v>10984.312861767999</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1659,7 +1659,7 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>1181.7796339624099</v>
+        <v>1525.5990085788901</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1667,7 +1667,7 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>61411.007724668103</v>
+        <v>106672.61314313899</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1675,7 +1675,7 @@
         <v>10</v>
       </c>
       <c r="B13">
-        <v>42904.5302275051</v>
+        <v>74526.351620319401</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1683,7 +1683,7 @@
         <v>11</v>
       </c>
       <c r="B14">
-        <v>13006.196953462701</v>
+        <v>24762.9427445076</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1691,7 +1691,7 @@
         <v>12</v>
       </c>
       <c r="B15">
-        <v>14898.889793705401</v>
+        <v>28366.5053080738</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1699,7 +1699,7 @@
         <v>13</v>
       </c>
       <c r="B16">
-        <v>11307.626455809001</v>
+        <v>21528.976341306799</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1707,7 +1707,7 @@
         <v>14</v>
       </c>
       <c r="B17">
-        <v>35621.4498650807</v>
+        <v>67820.895427121199</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1715,7 +1715,7 @@
         <v>15</v>
       </c>
       <c r="B18">
-        <v>9220.8112729772893</v>
+        <v>17555.8176173746</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1723,7 +1723,7 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <v>29361.0043165856</v>
+        <v>55901.419255324698</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1731,7 +1731,7 @@
         <v>17</v>
       </c>
       <c r="B20">
-        <v>89.328611872382496</v>
+        <v>13793.873527809101</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1739,7 +1739,7 @@
         <v>18</v>
       </c>
       <c r="B21">
-        <v>8832.5665877992997</v>
+        <v>16816.625296643</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>